<commit_message>
rejigging code to work in office
file paths changed in main
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregg_000\Documents\GitHub\RME_Rail_Fares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01621A3F-40CC-4051-B95C-C223D57E7CB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-225" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-225" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -133,12 +132,30 @@
   </si>
   <si>
     <t>0800,0830</t>
+  </si>
+  <si>
+    <t>Route 4</t>
+  </si>
+  <si>
+    <t>EUS,BHM</t>
+  </si>
+  <si>
+    <t>BHM,EUS</t>
+  </si>
+  <si>
+    <t>0900,1300,1600</t>
+  </si>
+  <si>
+    <t>0700,0800,0900</t>
+  </si>
+  <si>
+    <t>0600,1400,1500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,11 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +483,7 @@
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -479,8 +496,11 @@
       <c r="D1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -493,8 +513,11 @@
       <c r="D2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -507,8 +530,11 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -521,8 +547,11 @@
       <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -535,8 +564,11 @@
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -549,8 +581,11 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -563,8 +598,11 @@
       <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -577,8 +615,11 @@
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -590,6 +631,9 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new fields to output
Added date_different between date of collection and date of travel.  Added duration as well well
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -62,49 +62,67 @@
     <t>EDB,KGX</t>
   </si>
   <si>
-    <t>0612,0900,1000,1030,1200,1300,1330,1500,1530,1400,1900</t>
-  </si>
-  <si>
-    <t>0612,0830,0900,0930,1130,1200,1230,1430,1500,1530,1800</t>
-  </si>
-  <si>
-    <t>0848,0900,0930,1030,1100,1122,1230,1300,1330,1530,1600,1630,1900</t>
-  </si>
-  <si>
-    <t>0656,0830,0900,1030,1130,1400,1430,1530,1731,1830,1936</t>
-  </si>
-  <si>
-    <t>0626,0655,0930,1000,1130,1200,1330,1400,1630,1700</t>
-  </si>
-  <si>
-    <t>1030,1100,1430,1450,1630,1700,1800,1830</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
-  <si>
     <t>CMD,SRA</t>
   </si>
   <si>
     <t>SRA,CMD</t>
   </si>
   <si>
-    <t>0800,0900,1000</t>
-  </si>
-  <si>
-    <t>1100,1200,1315</t>
-  </si>
-  <si>
     <t>1600</t>
   </si>
   <si>
-    <t>1700,1730,1745</t>
-  </si>
-  <si>
-    <t>2000,2115</t>
-  </si>
-  <si>
     <t>1900</t>
+  </si>
+  <si>
+    <t>1030</t>
+  </si>
+  <si>
+    <t>0848</t>
+  </si>
+  <si>
+    <t>0612</t>
+  </si>
+  <si>
+    <t>0656</t>
+  </si>
+  <si>
+    <t>0626</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>0612,0700</t>
+  </si>
+  <si>
+    <t>0800,0900</t>
+  </si>
+  <si>
+    <t>Route2</t>
+  </si>
+  <si>
+    <t>Route3</t>
+  </si>
+  <si>
+    <t>EUS,LIV</t>
+  </si>
+  <si>
+    <t>LIV,EUS</t>
+  </si>
+  <si>
+    <t>1500,1700,1800</t>
+  </si>
+  <si>
+    <t>0900,1000,1100,1200</t>
+  </si>
+  <si>
+    <t>1300,1500,1612</t>
   </si>
 </sst>
 </file>
@@ -427,7 +445,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +464,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -457,7 +478,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -469,7 +493,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -478,12 +505,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -491,12 +520,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -504,12 +535,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -517,12 +550,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,12 +565,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,12 +580,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new routes and times
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -123,6 +123,33 @@
   </si>
   <si>
     <t>1300,1500,1612</t>
+  </si>
+  <si>
+    <t>Route4</t>
+  </si>
+  <si>
+    <t>WOK,WAT</t>
+  </si>
+  <si>
+    <t>WAT,WOK</t>
+  </si>
+  <si>
+    <t>1600,1730,1815</t>
+  </si>
+  <si>
+    <t>2300,0000</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>1100,1330</t>
+  </si>
+  <si>
+    <t>1215</t>
+  </si>
+  <si>
+    <t>0630,0700,0945,1100</t>
   </si>
 </sst>
 </file>
@@ -445,7 +472,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +481,7 @@
     <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,6 +497,9 @@
       <c r="D1" t="s">
         <v>27</v>
       </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -483,7 +514,9 @@
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -498,7 +531,9 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -513,7 +548,9 @@
       <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -528,7 +565,9 @@
       <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -543,7 +582,9 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -558,7 +599,9 @@
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -573,7 +616,9 @@
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -588,7 +633,9 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
live route data loaded
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -56,100 +56,127 @@
     <t>Route 1</t>
   </si>
   <si>
-    <t>KGX,EDB</t>
-  </si>
-  <si>
-    <t>EDB,KGX</t>
-  </si>
-  <si>
-    <t>CMD,SRA</t>
-  </si>
-  <si>
-    <t>SRA,CMD</t>
-  </si>
-  <si>
-    <t>1600</t>
-  </si>
-  <si>
-    <t>1900</t>
-  </si>
-  <si>
-    <t>1030</t>
-  </si>
-  <si>
-    <t>0848</t>
-  </si>
-  <si>
-    <t>0612</t>
-  </si>
-  <si>
-    <t>0656</t>
-  </si>
-  <si>
-    <t>0626</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>1700</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>0612,0700</t>
-  </si>
-  <si>
-    <t>0800,0900</t>
-  </si>
-  <si>
     <t>Route2</t>
   </si>
   <si>
     <t>Route3</t>
   </si>
   <si>
-    <t>EUS,LIV</t>
-  </si>
-  <si>
-    <t>LIV,EUS</t>
-  </si>
-  <si>
-    <t>1500,1700,1800</t>
-  </si>
-  <si>
-    <t>0900,1000,1100,1200</t>
-  </si>
-  <si>
-    <t>1300,1500,1612</t>
-  </si>
-  <si>
     <t>Route4</t>
   </si>
   <si>
-    <t>WOK,WAT</t>
-  </si>
-  <si>
-    <t>WAT,WOK</t>
-  </si>
-  <si>
-    <t>1600,1730,1815</t>
-  </si>
-  <si>
-    <t>2300,0000</t>
-  </si>
-  <si>
-    <t>1800</t>
-  </si>
-  <si>
-    <t>1100,1330</t>
-  </si>
-  <si>
-    <t>1215</t>
-  </si>
-  <si>
-    <t>0630,0700,0945,1100</t>
+    <t>DON,KGX</t>
+  </si>
+  <si>
+    <t>KGX,DON</t>
+  </si>
+  <si>
+    <t>GRA,KGX</t>
+  </si>
+  <si>
+    <t>CHD,STP</t>
+  </si>
+  <si>
+    <t>LEI,STP</t>
+  </si>
+  <si>
+    <t>YRK,KGX</t>
+  </si>
+  <si>
+    <t>LDS,KGX</t>
+  </si>
+  <si>
+    <t>0714,0717,0747,0831</t>
+  </si>
+  <si>
+    <t>0726,0801,0818</t>
+  </si>
+  <si>
+    <t>0701,0737,0742</t>
+  </si>
+  <si>
+    <t>0707,0755</t>
+  </si>
+  <si>
+    <t>0802,0821</t>
+  </si>
+  <si>
+    <t>0700,0740</t>
+  </si>
+  <si>
+    <t>1425,1430</t>
+  </si>
+  <si>
+    <t>1418,1501</t>
+  </si>
+  <si>
+    <t>14:13</t>
+  </si>
+  <si>
+    <t>14:03</t>
+  </si>
+  <si>
+    <t>13:51,13:57</t>
+  </si>
+  <si>
+    <t>14:15</t>
+  </si>
+  <si>
+    <t>1437,1528</t>
+  </si>
+  <si>
+    <t>1418,1412</t>
+  </si>
+  <si>
+    <t>1501</t>
+  </si>
+  <si>
+    <t>1417</t>
+  </si>
+  <si>
+    <t>1400,1552</t>
+  </si>
+  <si>
+    <t>1405</t>
+  </si>
+  <si>
+    <t>KGX,GRA</t>
+  </si>
+  <si>
+    <t>STP,CHD</t>
+  </si>
+  <si>
+    <t>STP,LEI</t>
+  </si>
+  <si>
+    <t>KGX,YRK</t>
+  </si>
+  <si>
+    <t>LGX,LDS</t>
+  </si>
+  <si>
+    <t>1627,16:30,17:03</t>
+  </si>
+  <si>
+    <t>1631,1702</t>
+  </si>
+  <si>
+    <t>1048,1103,1147</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>1448,1448,1550</t>
+  </si>
+  <si>
+    <t>1432</t>
+  </si>
+  <si>
+    <t>Route5</t>
+  </si>
+  <si>
+    <t>Route6</t>
   </si>
 </sst>
 </file>
@@ -469,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +511,7 @@
     <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -492,149 +519,173 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simple check for dud URLs
line 265 and 277 check for ""\\dep" in url string as sign of no times being supplied for route and/or day.
Metadata amended to remove NULL cells with a comma character
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -110,18 +111,6 @@
     <t>1418,1501</t>
   </si>
   <si>
-    <t>14:13</t>
-  </si>
-  <si>
-    <t>14:03</t>
-  </si>
-  <si>
-    <t>13:51,13:57</t>
-  </si>
-  <si>
-    <t>14:15</t>
-  </si>
-  <si>
     <t>1437,1528</t>
   </si>
   <si>
@@ -152,12 +141,6 @@
     <t>KGX,YRK</t>
   </si>
   <si>
-    <t>LGX,LDS</t>
-  </si>
-  <si>
-    <t>1627,16:30,17:03</t>
-  </si>
-  <si>
     <t>1631,1702</t>
   </si>
   <si>
@@ -177,6 +160,27 @@
   </si>
   <si>
     <t>Route6</t>
+  </si>
+  <si>
+    <t>1413</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>1351,1357</t>
+  </si>
+  <si>
+    <t>1415</t>
+  </si>
+  <si>
+    <t>1627,1630,1703</t>
+  </si>
+  <si>
+    <t>KGX,LDS</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -498,17 +502,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -528,10 +532,10 @@
         <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -542,19 +546,19 @@
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,16 +571,16 @@
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -585,39 +589,69 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -653,16 +687,16 @@
         <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -670,26 +704,89 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
attempts to build exe file - not very successful
</commit_message>
<xml_diff>
--- a/route_and_time_metadata.xlsx
+++ b/route_and_time_metadata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -181,30 +181,6 @@
   </si>
   <si>
     <t>1627,1630,1703, 2330</t>
-  </si>
-  <si>
-    <t>Route7</t>
-  </si>
-  <si>
-    <t>PAD,BRI</t>
-  </si>
-  <si>
-    <t>BRI,PAD</t>
-  </si>
-  <si>
-    <t>0730,0800</t>
-  </si>
-  <si>
-    <t>1230,1300,2300</t>
-  </si>
-  <si>
-    <t>1930,2000</t>
-  </si>
-  <si>
-    <t>2300,2330</t>
-  </si>
-  <si>
-    <t>1730,1845</t>
   </si>
 </sst>
 </file>
@@ -527,7 +503,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,9 +537,6 @@
       <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -587,9 +560,6 @@
       <c r="G2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -613,9 +583,6 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -639,9 +606,7 @@
       <c r="G4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -665,9 +630,7 @@
       <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -691,9 +654,7 @@
       <c r="G6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -717,9 +678,7 @@
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -743,9 +702,7 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -768,9 +725,6 @@
       </c>
       <c r="G9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>